<commit_message>
Baselined from internal Repository last_commit:a3536a8b09f775b1ce4521a149f408efdecde48e
</commit_message>
<xml_diff>
--- a/src/configs/input_excel_example.xlsx
+++ b/src/configs/input_excel_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmaco/Documents/DevNet/Case_Work/gve_devnet_meraki_org_day0_network_setup/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556CB6D8-860E-9F42-ABAE-20B9C30057F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16D6111-7CF5-DF48-B366-1400375F5D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19800" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
+    <workbookView xWindow="39000" yWindow="2220" windowWidth="38400" windowHeight="19700" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
   </bookViews>
   <sheets>
     <sheet name="CODING" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="45">
   <si>
     <t>Name of the Network</t>
   </si>
@@ -165,13 +165,19 @@
   </si>
   <si>
     <t>1000000  &lt;download - remove!&gt;</t>
+  </si>
+  <si>
+    <t>Note: Everything before "Networks" will no be processed! (allows defining global cells to reference)</t>
+  </si>
+  <si>
+    <t>Networks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,6 +210,14 @@
       <name val="Cambria Math"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -225,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -299,11 +313,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -343,6 +368,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,7 +691,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC04531-48DF-F741-8C2F-1512D0028C1C}">
-  <dimension ref="A1:K1048546"/>
+  <dimension ref="A1:K1048557"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -675,366 +709,139 @@
     <col min="10" max="10" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+    </row>
+    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>100</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>150</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>192</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>200</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1042,13 +849,20 @@
       <c r="I17" s="6"/>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1056,17 +870,15 @@
       <c r="I18" s="6"/>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1074,271 +886,535 @@
       <c r="I19" s="6"/>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>100</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>150</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>192</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>200</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="D31" s="11"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="13"/>
+    </row>
+    <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="13"/>
+    </row>
+    <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="4" t="e">
+      <c r="D33" s="4" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J35" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>1</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="5" t="b">
+      <c r="E36" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>100</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="5" t="b">
+      <c r="E37" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H37" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J37" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="38" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
         <v>150</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="5" t="b">
+      <c r="E38" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G38" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H38" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J38" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="39" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
         <v>192</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="5" t="b">
+      <c r="E39" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I39" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J39" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+    <row r="40" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
         <v>200</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="5" t="b">
+      <c r="E40" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I40" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J40" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="1048546" spans="3:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="C1048546" s="4"/>
-      <c r="E1048546" s="4"/>
+    <row r="1048557" spans="3:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="C1048557" s="4"/>
+      <c r="E1048557" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:I11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Baselined from internal Repository last_commit:a4afae663847394daf308c15f749e128f2555d99
</commit_message>
<xml_diff>
--- a/src/configs/input_excel_example.xlsx
+++ b/src/configs/input_excel_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmaco/Documents/DevNet/Case_Work/gve_devnet_meraki_org_day0_network_setup/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16D6111-7CF5-DF48-B366-1400375F5D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AEE488-25A5-C848-BC80-A764DEC54D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39000" yWindow="2220" windowWidth="38400" windowHeight="19700" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
+    <workbookView xWindow="38400" yWindow="1900" windowWidth="38400" windowHeight="19700" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
   </bookViews>
   <sheets>
     <sheet name="CODING" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
   <si>
     <t>Name of the Network</t>
   </si>
@@ -171,13 +171,37 @@
   </si>
   <si>
     <t>Networks</t>
+  </si>
+  <si>
+    <t>MX Port ID</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>VLAN</t>
+  </si>
+  <si>
+    <t>Access Policy</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>MX 18.107.9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,8 +242,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +273,12 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -328,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -368,11 +411,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -691,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC04531-48DF-F741-8C2F-1512D0028C1C}">
-  <dimension ref="A1:K1048557"/>
+  <dimension ref="A1:K1048560"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,10 +765,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -727,25 +782,27 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -859,9 +916,9 @@
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="4" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D18" s="4" t="str">
+        <f>A3</f>
+        <v>MX 18.107.9</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
@@ -1072,91 +1129,107 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="A26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="12"/>
+      <c r="A27" s="3">
+        <v>4</v>
+      </c>
+      <c r="B27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="4">
+        <v>100</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="19"/>
     </row>
     <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="3">
+        <v>5</v>
+      </c>
+      <c r="B28" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="13"/>
+      <c r="C28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="4">
+        <v>100</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="13"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="12"/>
     </row>
     <row r="31" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -1166,17 +1239,11 @@
     </row>
     <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
@@ -1186,18 +1253,15 @@
     </row>
     <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="4" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -1207,13 +1271,15 @@
     </row>
     <row r="34" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="11"/>
       <c r="E34" s="6"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
@@ -1223,131 +1289,100 @@
     </row>
     <row r="35" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <f>A3</f>
+        <v>MX 18.107.9</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I38" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="J38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
-        <v>1</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <v>100</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
-        <v>150</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>20</v>
@@ -1359,27 +1394,19 @@
         <v>0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
     </row>
     <row r="40" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>20</v>
@@ -1406,9 +1433,105 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1048557" spans="3:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="C1048557" s="4"/>
-      <c r="E1048557" s="4"/>
+    <row r="41" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>150</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>192</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>200</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1048560" spans="3:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="C1048560" s="4"/>
+      <c r="E1048560" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Baselined from internal Repository last_commit:fec2fe0705aa5da8a1add065a159c0fa4f8c70ba
</commit_message>
<xml_diff>
--- a/src/configs/input_excel_example.xlsx
+++ b/src/configs/input_excel_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmaco/Documents/DevNet/Case_Work/gve_devnet_meraki_org_day0_network_setup/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AEE488-25A5-C848-BC80-A764DEC54D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D299B96A-4479-3144-9170-B1AF71D9F511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1900" windowWidth="38400" windowHeight="19700" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
   </bookViews>
   <sheets>
     <sheet name="CODING" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="62">
   <si>
     <t>Name of the Network</t>
   </si>
@@ -195,6 +195,33 @@
   </si>
   <si>
     <t>MX 18.107.9</t>
+  </si>
+  <si>
+    <t>Warm Spare Serial</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>uplinkMode</t>
+  </si>
+  <si>
+    <t>virtualIp1</t>
+  </si>
+  <si>
+    <t>virtualIp2</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>Template Name</t>
+  </si>
+  <si>
+    <t>retainConfigs</t>
+  </si>
+  <si>
+    <t>&lt;Template Name&gt;</t>
   </si>
 </sst>
 </file>
@@ -282,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -367,11 +394,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -416,10 +487,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -432,6 +499,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC04531-48DF-F741-8C2F-1512D0028C1C}">
-  <dimension ref="A1:K1048560"/>
+  <dimension ref="A1:K1048564"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,10 +850,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -792,17 +877,17 @@
       <c r="A4" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -820,46 +905,44 @@
       <c r="I12" s="8"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>59</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="4"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="13"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
@@ -870,15 +953,11 @@
     </row>
     <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -888,17 +967,15 @@
     </row>
     <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -908,18 +985,15 @@
     </row>
     <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <f>A3</f>
-        <v>MX 18.107.9</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="11"/>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -929,13 +1003,17 @@
     </row>
     <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -945,99 +1023,80 @@
     </row>
     <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4" t="str">
+        <f>A3</f>
+        <v>MX 18.107.9</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>1</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>100</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>150</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>20</v>
@@ -1046,30 +1105,22 @@
         <v>21</v>
       </c>
       <c r="E23" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
-        <v>192</v>
+        <v>100</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
@@ -1078,13 +1129,13 @@
         <v>21</v>
       </c>
       <c r="E24" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>24</v>
@@ -1098,10 +1149,10 @@
     </row>
     <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>20</v>
@@ -1129,177 +1180,211 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
+      <c r="A26" s="3">
+        <v>192</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
+        <v>200</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="28"/>
+    </row>
+    <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <v>4</v>
       </c>
-      <c r="B27" s="4" t="b">
+      <c r="B29" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D29" s="4">
         <v>100</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="19"/>
-    </row>
-    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="F29" s="29"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>5</v>
       </c>
-      <c r="B28" s="4" t="b">
+      <c r="B30" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D30" s="4">
         <v>100</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-    </row>
-    <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="12"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="29"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="30"/>
+    </row>
+    <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="13"/>
+      <c r="C32" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="31"/>
     </row>
     <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="13"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="12"/>
     </row>
     <row r="35" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -1309,18 +1394,11 @@
     </row>
     <row r="36" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="4" t="str">
-        <f>A3</f>
-        <v>MX 18.107.9</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -1330,13 +1408,15 @@
     </row>
     <row r="37" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -1346,163 +1426,118 @@
     </row>
     <row r="38" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="4" t="str">
+        <f>A3</f>
+        <v>MX 18.107.9</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="13"/>
+    </row>
+    <row r="41" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="13"/>
+    </row>
+    <row r="42" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I42" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <v>1</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <v>100</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
-        <v>150</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <v>192</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="K42" s="1"/>
     </row>
     <row r="43" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>20</v>
@@ -1511,27 +1546,147 @@
         <v>21</v>
       </c>
       <c r="E43" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>100</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H44" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I44" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="J44" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="1048560" spans="3:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="C1048560" s="4"/>
-      <c r="E1048560" s="4"/>
+    <row r="45" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>150</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>192</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>200</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1048564" spans="3:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="C1048564" s="4"/>
+      <c r="E1048564" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Baselined from internal Repository last_commit:a09f3286eea5a01f6d0600c8f87498a4e8137ac1
</commit_message>
<xml_diff>
--- a/src/configs/input_excel_example.xlsx
+++ b/src/configs/input_excel_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmaco/Documents/DevNet/Case_Work/gve_devnet_meraki_org_day0_network_setup/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D299B96A-4479-3144-9170-B1AF71D9F511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FD110B-C3CA-8243-9C61-6279A9C0269C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="63">
   <si>
     <t>Name of the Network</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>&lt;Template Name&gt;</t>
+  </si>
+  <si>
+    <t>YYYY-YYYY-YYYY</t>
   </si>
 </sst>
 </file>
@@ -491,6 +494,24 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -499,24 +520,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC04531-48DF-F741-8C2F-1512D0028C1C}">
-  <dimension ref="A1:K1048564"/>
+  <dimension ref="A1:K1048565"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,10 +853,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -877,17 +880,17 @@
       <c r="A4" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1044,13 +1047,18 @@
     </row>
     <row r="21" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4" t="str">
+        <f>A3</f>
+        <v>MX 18.107.9</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1060,67 +1068,59 @@
     </row>
     <row r="22" spans="1:11" ht="21" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>1</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <v>100</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>20</v>
@@ -1129,30 +1129,22 @@
         <v>21</v>
       </c>
       <c r="E24" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>20</v>
@@ -1181,10 +1173,10 @@
     </row>
     <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
-        <v>192</v>
+        <v>150</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>20</v>
@@ -1193,13 +1185,13 @@
         <v>21</v>
       </c>
       <c r="E26" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>24</v>
@@ -1213,10 +1205,10 @@
     </row>
     <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>20</v>
@@ -1225,71 +1217,81 @@
         <v>21</v>
       </c>
       <c r="E27" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>200</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F28" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G28" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="26" t="s">
+      <c r="H28" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="I27" s="26" t="s">
+      <c r="I28" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J28" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="28"/>
-    </row>
-    <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>4</v>
-      </c>
-      <c r="B29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="4">
-        <v>100</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="30"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="24"/>
     </row>
     <row r="30" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" s="4" t="b">
         <v>1</v>
@@ -1303,100 +1305,108 @@
       <c r="E30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="30"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="3">
+        <v>5</v>
+      </c>
+      <c r="B31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="4">
+        <v>100</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="30"/>
-    </row>
-    <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="4" t="b">
+      <c r="F32" s="25"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="26"/>
+    </row>
+    <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="31"/>
-    </row>
-    <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="27"/>
     </row>
     <row r="34" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="12"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1408,14 +1418,10 @@
     </row>
     <row r="37" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="7"/>
@@ -1426,15 +1432,15 @@
     </row>
     <row r="38" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="11"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
@@ -1444,17 +1450,15 @@
     </row>
     <row r="39" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="11"/>
       <c r="E39" s="6"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -1464,17 +1468,16 @@
     </row>
     <row r="40" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="4" t="str">
-        <f>A3</f>
-        <v>MX 18.107.9</v>
+        <v>15</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="7"/>
@@ -1485,13 +1488,18 @@
     </row>
     <row r="41" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="4" t="str">
+        <f>A3</f>
+        <v>MX 18.107.9</v>
+      </c>
       <c r="E41" s="6"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -1501,67 +1509,59 @@
     </row>
     <row r="42" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E43" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="I43" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="J43" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <v>1</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
+      <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>20</v>
@@ -1570,30 +1570,22 @@
         <v>21</v>
       </c>
       <c r="E44" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
     </row>
     <row r="45" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>20</v>
@@ -1622,10 +1614,10 @@
     </row>
     <row r="46" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
-        <v>192</v>
+        <v>150</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>20</v>
@@ -1634,13 +1626,13 @@
         <v>21</v>
       </c>
       <c r="E46" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>24</v>
@@ -1654,10 +1646,10 @@
     </row>
     <row r="47" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>20</v>
@@ -1666,13 +1658,13 @@
         <v>21</v>
       </c>
       <c r="E47" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>24</v>
@@ -1684,9 +1676,41 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1048564" spans="3:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="C1048564" s="4"/>
-      <c r="E1048564" s="4"/>
+    <row r="48" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>200</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1048565" spans="3:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="C1048565" s="4"/>
+      <c r="E1048565" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Baselined from internal Repository last_commit:febb30503c0b2cf936d320136e495c1f901bdb6c
</commit_message>
<xml_diff>
--- a/src/configs/input_excel_example.xlsx
+++ b/src/configs/input_excel_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmaco/Documents/DevNet/Case_Work/gve_devnet_meraki_org_day0_network_setup/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FD110B-C3CA-8243-9C61-6279A9C0269C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D6ABF8-1CDB-B542-9B18-5DF367BCB14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20720" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
+    <workbookView xWindow="1620" yWindow="780" windowWidth="35840" windowHeight="19880" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
   </bookViews>
   <sheets>
     <sheet name="CODING" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
   <si>
     <t>Name of the Network</t>
   </si>
@@ -176,18 +176,6 @@
     <t>MX Port ID</t>
   </si>
   <si>
-    <t>Enabled</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>VLAN</t>
-  </si>
-  <si>
-    <t>Access Policy</t>
-  </si>
-  <si>
     <t>Access</t>
   </si>
   <si>
@@ -225,6 +213,15 @@
   </si>
   <si>
     <t>YYYY-YYYY-YYYY</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>vlan</t>
+  </si>
+  <si>
+    <t>accessPolicy</t>
   </si>
 </sst>
 </file>
@@ -836,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC04531-48DF-F741-8C2F-1512D0028C1C}">
   <dimension ref="A1:K1048565"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -871,7 +868,7 @@
     </row>
     <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -910,10 +907,10 @@
     </row>
     <row r="13" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -925,7 +922,7 @@
     </row>
     <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B14" s="4" t="b">
         <v>0</v>
@@ -1050,7 +1047,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>14</v>
@@ -1272,16 +1269,16 @@
         <v>45</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F29" s="23"/>
       <c r="G29" s="17"/>
@@ -1297,13 +1294,13 @@
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D30" s="4">
         <v>100</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F30" s="25"/>
       <c r="G30" s="21"/>
@@ -1319,13 +1316,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D31" s="4">
         <v>100</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F31" s="25"/>
       <c r="G31" s="21"/>
@@ -1335,19 +1332,19 @@
     </row>
     <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="F32" s="25"/>
       <c r="G32" s="21"/>
@@ -1357,13 +1354,13 @@
     </row>
     <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B33" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="5"/>

</xml_diff>

<commit_message>
Baselined from internal Repository last_commit:8e29f6bbd1facadaab31b3e023a68fbf03b42ac6
</commit_message>
<xml_diff>
--- a/src/configs/input_excel_example.xlsx
+++ b/src/configs/input_excel_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmaco/Documents/DevNet/Case_Work/gve_devnet_meraki_org_day0_network_setup/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D6ABF8-1CDB-B542-9B18-5DF367BCB14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7B9F54-B7A7-2E45-B21C-C90A895C1AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="780" windowWidth="35840" windowHeight="19880" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
   </bookViews>
   <sheets>
     <sheet name="CODING" sheetId="2" r:id="rId1"/>
@@ -228,38 +228,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Cambria Math"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Cambria Math"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="9"/>
-      <name val="Cambria Math"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Cambria Math"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -271,19 +246,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria Math"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,20 +261,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD0CECE"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -357,26 +314,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -410,6 +347,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -420,6 +370,15 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -432,7 +391,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -442,81 +403,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,177 +754,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC04531-48DF-F741-8C2F-1512D0028C1C}">
-  <dimension ref="A1:K1048565"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="55.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
-    <col min="4" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="33.5" customWidth="1"/>
-    <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="9" width="31.5" customWidth="1"/>
-    <col min="10" max="10" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10.6640625" style="1"/>
+    <col min="15" max="15" width="10.6640625" style="24"/>
+    <col min="16" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="29"/>
-    </row>
-    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-    </row>
-    <row r="11" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-    </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="12"/>
-    </row>
-    <row r="13" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="4" t="b">
+      <c r="B14" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="13"/>
-    </row>
-    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D17" s="9"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D18" s="9"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -1011,17 +1041,17 @@
       <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="E19" s="9"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -1031,92 +1061,91 @@
       <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="4" t="str">
+      <c r="D20" s="6" t="str">
         <f>A3</f>
         <v>MX 18.107.9</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="E20" s="9"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="4" t="str">
+      <c r="D21" s="12" t="str">
         <f>A3</f>
         <v>MX 18.107.9</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="E21" s="9"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>1</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -1125,22 +1154,18 @@
       <c r="D24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="5" t="b">
+      <c r="E24" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <v>100</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1149,7 +1174,7 @@
       <c r="D25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="5" t="b">
+      <c r="E25" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1164,15 +1189,15 @@
       <c r="I25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
         <v>150</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1181,7 +1206,7 @@
       <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="5" t="b">
+      <c r="E26" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -1196,15 +1221,15 @@
       <c r="I26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
         <v>192</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1213,7 +1238,7 @@
       <c r="D27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="5" t="b">
+      <c r="E27" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1228,15 +1253,15 @@
       <c r="I27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
         <v>200</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1245,26 +1270,26 @@
       <c r="D28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="5" t="b">
+      <c r="E28" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
@@ -1277,16 +1302,16 @@
       <c r="D29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="24"/>
-    </row>
-    <row r="30" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="9"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>4</v>
       </c>
@@ -1299,16 +1324,16 @@
       <c r="D30" s="4">
         <v>100</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="26"/>
-    </row>
-    <row r="31" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="9"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>5</v>
       </c>
@@ -1321,16 +1346,16 @@
       <c r="D31" s="4">
         <v>100</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="26"/>
-    </row>
-    <row r="32" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="9"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
@@ -1343,16 +1368,16 @@
       <c r="D32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="26"/>
-    </row>
-    <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F32" s="9"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>58</v>
       </c>
@@ -1363,71 +1388,72 @@
         <v>54</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="27"/>
-    </row>
-    <row r="34" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E33" s="6"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="8"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="12"/>
-    </row>
-    <row r="36" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="13"/>
-    </row>
-    <row r="37" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="9"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="4"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="13"/>
-    </row>
-    <row r="38" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="9"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
@@ -1437,15 +1463,15 @@
       <c r="C38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="13"/>
-    </row>
-    <row r="39" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D38" s="9"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>3</v>
       </c>
@@ -1455,72 +1481,72 @@
       <c r="C39" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="13"/>
-    </row>
-    <row r="40" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="9"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="13"/>
-    </row>
-    <row r="41" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E40" s="9"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="4" t="str">
         <f>A3</f>
         <v>MX 18.107.9</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="13"/>
-    </row>
-    <row r="42" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E41" s="9"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="13"/>
-    </row>
-    <row r="43" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="17"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>33</v>
       </c>
@@ -1533,7 +1559,7 @@
       <c r="D43" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="3" t="s">
         <v>34</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -1548,16 +1574,15 @@
       <c r="I43" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J43" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>1</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -1566,22 +1591,18 @@
       <c r="D44" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="5" t="b">
+      <c r="E44" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>100</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -1590,7 +1611,7 @@
       <c r="D45" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="5" t="b">
+      <c r="E45" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F45" s="4" t="s">
@@ -1605,15 +1626,15 @@
       <c r="I45" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="J45" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>150</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -1622,7 +1643,7 @@
       <c r="D46" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="5" t="b">
+      <c r="E46" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
@@ -1637,15 +1658,15 @@
       <c r="I46" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J46" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>192</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -1654,7 +1675,7 @@
       <c r="D47" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="5" t="b">
+      <c r="E47" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -1669,15 +1690,15 @@
       <c r="I47" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J47" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>200</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -1686,7 +1707,7 @@
       <c r="D48" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="5" t="b">
+      <c r="E48" s="4" t="b">
         <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -1701,19 +1722,330 @@
       <c r="I48" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="1048565" spans="3:5" ht="21" x14ac:dyDescent="0.2">
-      <c r="C1048565" s="4"/>
-      <c r="E1048565" s="4"/>
+    <row r="49" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="25"/>
+    </row>
+    <row r="50" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+    </row>
+    <row r="51" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+    </row>
+    <row r="52" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+    </row>
+    <row r="53" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+    </row>
+    <row r="54" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+    </row>
+    <row r="55" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+    </row>
+    <row r="56" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K56" s="25"/>
+      <c r="L56" s="25"/>
+      <c r="M56" s="25"/>
+      <c r="N56" s="25"/>
+    </row>
+    <row r="57" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K57" s="25"/>
+      <c r="L57" s="25"/>
+      <c r="M57" s="25"/>
+      <c r="N57" s="25"/>
+    </row>
+    <row r="58" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K58" s="25"/>
+      <c r="L58" s="25"/>
+      <c r="M58" s="25"/>
+      <c r="N58" s="25"/>
+    </row>
+    <row r="59" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K59" s="25"/>
+      <c r="L59" s="25"/>
+      <c r="M59" s="25"/>
+      <c r="N59" s="25"/>
+    </row>
+    <row r="60" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K60" s="25"/>
+      <c r="L60" s="25"/>
+      <c r="M60" s="25"/>
+      <c r="N60" s="25"/>
+    </row>
+    <row r="61" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K61" s="25"/>
+      <c r="L61" s="25"/>
+      <c r="M61" s="25"/>
+      <c r="N61" s="25"/>
+    </row>
+    <row r="62" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K62" s="25"/>
+      <c r="L62" s="25"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="25"/>
+    </row>
+    <row r="63" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K63" s="25"/>
+      <c r="L63" s="25"/>
+      <c r="M63" s="25"/>
+      <c r="N63" s="25"/>
+    </row>
+    <row r="64" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K64" s="25"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="25"/>
+    </row>
+    <row r="65" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K65" s="25"/>
+      <c r="L65" s="25"/>
+      <c r="M65" s="25"/>
+      <c r="N65" s="25"/>
+    </row>
+    <row r="66" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K66" s="25"/>
+      <c r="L66" s="25"/>
+      <c r="M66" s="25"/>
+      <c r="N66" s="25"/>
+    </row>
+    <row r="67" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K67" s="25"/>
+      <c r="L67" s="25"/>
+      <c r="M67" s="25"/>
+      <c r="N67" s="25"/>
+    </row>
+    <row r="68" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K68" s="25"/>
+      <c r="L68" s="25"/>
+      <c r="M68" s="25"/>
+      <c r="N68" s="25"/>
+    </row>
+    <row r="69" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K69" s="25"/>
+      <c r="L69" s="25"/>
+      <c r="M69" s="25"/>
+      <c r="N69" s="25"/>
+    </row>
+    <row r="70" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K70" s="25"/>
+      <c r="L70" s="25"/>
+      <c r="M70" s="25"/>
+      <c r="N70" s="25"/>
+    </row>
+    <row r="71" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K71" s="25"/>
+      <c r="L71" s="25"/>
+      <c r="M71" s="25"/>
+      <c r="N71" s="25"/>
+    </row>
+    <row r="72" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K72" s="25"/>
+      <c r="L72" s="25"/>
+      <c r="M72" s="25"/>
+      <c r="N72" s="25"/>
+    </row>
+    <row r="73" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K73" s="25"/>
+      <c r="L73" s="25"/>
+      <c r="M73" s="25"/>
+      <c r="N73" s="25"/>
+    </row>
+    <row r="74" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K74" s="25"/>
+      <c r="L74" s="25"/>
+      <c r="M74" s="25"/>
+      <c r="N74" s="25"/>
+    </row>
+    <row r="75" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K75" s="25"/>
+      <c r="L75" s="25"/>
+      <c r="M75" s="25"/>
+      <c r="N75" s="25"/>
+    </row>
+    <row r="76" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K76" s="25"/>
+      <c r="L76" s="25"/>
+      <c r="M76" s="25"/>
+      <c r="N76" s="25"/>
+    </row>
+    <row r="77" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K77" s="25"/>
+      <c r="L77" s="25"/>
+      <c r="M77" s="25"/>
+      <c r="N77" s="25"/>
+    </row>
+    <row r="78" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K78" s="25"/>
+      <c r="L78" s="25"/>
+      <c r="M78" s="25"/>
+      <c r="N78" s="25"/>
+    </row>
+    <row r="79" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K79" s="25"/>
+      <c r="L79" s="25"/>
+      <c r="M79" s="25"/>
+      <c r="N79" s="25"/>
+    </row>
+    <row r="80" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K80" s="25"/>
+      <c r="L80" s="25"/>
+      <c r="M80" s="25"/>
+      <c r="N80" s="25"/>
+    </row>
+    <row r="81" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K81" s="25"/>
+      <c r="L81" s="25"/>
+      <c r="M81" s="25"/>
+      <c r="N81" s="25"/>
+    </row>
+    <row r="82" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K82" s="25"/>
+      <c r="L82" s="25"/>
+      <c r="M82" s="25"/>
+      <c r="N82" s="25"/>
+    </row>
+    <row r="83" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K83" s="25"/>
+      <c r="L83" s="25"/>
+      <c r="M83" s="25"/>
+      <c r="N83" s="25"/>
+    </row>
+    <row r="84" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K84" s="25"/>
+      <c r="L84" s="25"/>
+      <c r="M84" s="25"/>
+      <c r="N84" s="25"/>
+    </row>
+    <row r="85" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K85" s="25"/>
+      <c r="L85" s="25"/>
+      <c r="M85" s="25"/>
+      <c r="N85" s="25"/>
+    </row>
+    <row r="86" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K86" s="25"/>
+      <c r="L86" s="25"/>
+      <c r="M86" s="25"/>
+      <c r="N86" s="25"/>
+    </row>
+    <row r="87" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K87" s="25"/>
+      <c r="L87" s="25"/>
+      <c r="M87" s="25"/>
+      <c r="N87" s="25"/>
+    </row>
+    <row r="88" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K88" s="25"/>
+      <c r="L88" s="25"/>
+      <c r="M88" s="25"/>
+      <c r="N88" s="25"/>
+    </row>
+    <row r="89" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K89" s="25"/>
+      <c r="L89" s="25"/>
+      <c r="M89" s="25"/>
+      <c r="N89" s="25"/>
+    </row>
+    <row r="90" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K90" s="25"/>
+      <c r="L90" s="25"/>
+      <c r="M90" s="25"/>
+      <c r="N90" s="25"/>
+    </row>
+    <row r="91" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K91" s="25"/>
+      <c r="L91" s="25"/>
+      <c r="M91" s="25"/>
+      <c r="N91" s="25"/>
+    </row>
+    <row r="92" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K92" s="25"/>
+      <c r="L92" s="25"/>
+      <c r="M92" s="25"/>
+      <c r="N92" s="25"/>
+    </row>
+    <row r="93" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K93" s="25"/>
+      <c r="L93" s="25"/>
+      <c r="M93" s="25"/>
+      <c r="N93" s="25"/>
+    </row>
+    <row r="94" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K94" s="25"/>
+      <c r="L94" s="25"/>
+      <c r="M94" s="25"/>
+      <c r="N94" s="25"/>
+    </row>
+    <row r="95" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K95" s="25"/>
+      <c r="L95" s="25"/>
+      <c r="M95" s="25"/>
+      <c r="N95" s="25"/>
+    </row>
+    <row r="96" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K96" s="25"/>
+      <c r="L96" s="25"/>
+      <c r="M96" s="25"/>
+      <c r="N96" s="25"/>
+    </row>
+    <row r="97" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K97" s="25"/>
+      <c r="L97" s="25"/>
+      <c r="M97" s="25"/>
+      <c r="N97" s="25"/>
+    </row>
+    <row r="98" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K98" s="25"/>
+      <c r="L98" s="25"/>
+      <c r="M98" s="25"/>
+      <c r="N98" s="25"/>
+    </row>
+    <row r="99" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K99" s="25"/>
+      <c r="L99" s="25"/>
+      <c r="M99" s="25"/>
+      <c r="N99" s="25"/>
+    </row>
+    <row r="100" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K100" s="25"/>
+      <c r="L100" s="25"/>
+      <c r="M100" s="25"/>
+      <c r="N100" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:I11"/>
+  <mergeCells count="1">
+    <mergeCell ref="A11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Cisco Confidential</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Baselined from internal Repository last_commit:30e38c422573b0980c24d263c59033f3cdfcaa9f
</commit_message>
<xml_diff>
--- a/src/configs/input_excel_example.xlsx
+++ b/src/configs/input_excel_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmaco/Documents/DevNet/Case_Work/gve_devnet_meraki_org_day0_network_setup/src/configs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7B9F54-B7A7-2E45-B21C-C90A895C1AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2359ECA6-F474-D64D-948E-C295812DC674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{D86E5BCB-62A3-6240-A2F0-41300153094C}"/>
   </bookViews>
   <sheets>
     <sheet name="CODING" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="74">
   <si>
     <t>Name of the Network</t>
   </si>
@@ -222,13 +222,49 @@
   </si>
   <si>
     <t>accessPolicy</t>
+  </si>
+  <si>
+    <t>Device Settings (Uplink)</t>
+  </si>
+  <si>
+    <t>svis</t>
+  </si>
+  <si>
+    <t>assignmentMode</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>gateway</t>
+  </si>
+  <si>
+    <t>nameservers</t>
+  </si>
+  <si>
+    <t>wan1</t>
+  </si>
+  <si>
+    <t>ipv4</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>X.X.X.X/24</t>
+  </si>
+  <si>
+    <t>X.X.X.X</t>
+  </si>
+  <si>
+    <t>wan2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -251,6 +287,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -266,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -399,11 +442,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -426,6 +502,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,8 +521,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC04531-48DF-F741-8C2F-1512D0028C1C}">
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,7 +855,7 @@
     <col min="9" max="9" width="30.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="10.6640625" style="1"/>
-    <col min="15" max="15" width="10.6640625" style="24"/>
+    <col min="15" max="15" width="10.6640625" style="20"/>
     <col min="16" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
@@ -904,18 +986,18 @@
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1073,7 +1155,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1094,143 +1176,137 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>67</v>
+      </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="31"/>
+      <c r="B23" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="23"/>
+      <c r="B24" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C26" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G26" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H26" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I26" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J26" s="19" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>1</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
-        <v>100</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
-        <v>150</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>20</v>
@@ -1242,27 +1318,15 @@
         <v>0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>20</v>
@@ -1273,103 +1337,133 @@
       <c r="E28" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="A29" s="5">
+        <v>150</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>4</v>
-      </c>
-      <c r="B30" s="4" t="b">
+      <c r="A30" s="5">
+        <v>192</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>200</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="4">
-        <v>100</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>5</v>
-      </c>
-      <c r="B31" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="4">
-        <v>100</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="F31" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="8"/>
@@ -1378,92 +1472,110 @@
       <c r="J32" s="8"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>58</v>
+      <c r="A33" s="3">
+        <v>4</v>
       </c>
       <c r="B33" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
+        <v>46</v>
+      </c>
+      <c r="D33" s="4">
+        <v>100</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
+      <c r="A34" s="3">
+        <v>5</v>
+      </c>
+      <c r="B34" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="4">
+        <v>100</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="9"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="C36" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
@@ -1473,15 +1585,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -1491,18 +1601,12 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -1511,19 +1615,16 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="4" t="str">
-        <f>A3</f>
-        <v>MX 18.107.9</v>
-      </c>
-      <c r="E41" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -1532,13 +1633,15 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
+        <v>41</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="9"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
@@ -1548,126 +1651,99 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="4" t="str">
+        <f>A3</f>
+        <v>MX 18.107.9</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H46" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="I46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J43" s="7" t="s">
+      <c r="J46" s="7" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <v>1</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <v>100</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
-        <v>150</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
-        <v>192</v>
+        <v>1</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>20</v>
@@ -1679,27 +1755,15 @@
         <v>0</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>20</v>
@@ -1726,318 +1790,154 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
-    </row>
-    <row r="50" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="25"/>
-    </row>
-    <row r="51" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K51" s="25"/>
-      <c r="L51" s="25"/>
-      <c r="M51" s="25"/>
-      <c r="N51" s="25"/>
-    </row>
-    <row r="52" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-    </row>
-    <row r="53" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-    </row>
-    <row r="54" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-    </row>
-    <row r="55" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K55" s="25"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="25"/>
-    </row>
-    <row r="56" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K56" s="25"/>
-      <c r="L56" s="25"/>
-      <c r="M56" s="25"/>
-      <c r="N56" s="25"/>
-    </row>
-    <row r="57" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K57" s="25"/>
-      <c r="L57" s="25"/>
-      <c r="M57" s="25"/>
-      <c r="N57" s="25"/>
-    </row>
-    <row r="58" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K58" s="25"/>
-      <c r="L58" s="25"/>
-      <c r="M58" s="25"/>
-      <c r="N58" s="25"/>
-    </row>
-    <row r="59" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K59" s="25"/>
-      <c r="L59" s="25"/>
-      <c r="M59" s="25"/>
-      <c r="N59" s="25"/>
-    </row>
-    <row r="60" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K60" s="25"/>
-      <c r="L60" s="25"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="25"/>
-    </row>
-    <row r="61" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K61" s="25"/>
-      <c r="L61" s="25"/>
-      <c r="M61" s="25"/>
-      <c r="N61" s="25"/>
-    </row>
-    <row r="62" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K62" s="25"/>
-      <c r="L62" s="25"/>
-      <c r="M62" s="25"/>
-      <c r="N62" s="25"/>
-    </row>
-    <row r="63" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K63" s="25"/>
-      <c r="L63" s="25"/>
-      <c r="M63" s="25"/>
-      <c r="N63" s="25"/>
-    </row>
-    <row r="64" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K64" s="25"/>
-      <c r="L64" s="25"/>
-      <c r="M64" s="25"/>
-      <c r="N64" s="25"/>
-    </row>
-    <row r="65" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K65" s="25"/>
-      <c r="L65" s="25"/>
-      <c r="M65" s="25"/>
-      <c r="N65" s="25"/>
-    </row>
-    <row r="66" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K66" s="25"/>
-      <c r="L66" s="25"/>
-      <c r="M66" s="25"/>
-      <c r="N66" s="25"/>
-    </row>
-    <row r="67" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K67" s="25"/>
-      <c r="L67" s="25"/>
-      <c r="M67" s="25"/>
-      <c r="N67" s="25"/>
-    </row>
-    <row r="68" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K68" s="25"/>
-      <c r="L68" s="25"/>
-      <c r="M68" s="25"/>
-      <c r="N68" s="25"/>
-    </row>
-    <row r="69" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K69" s="25"/>
-      <c r="L69" s="25"/>
-      <c r="M69" s="25"/>
-      <c r="N69" s="25"/>
-    </row>
-    <row r="70" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K70" s="25"/>
-      <c r="L70" s="25"/>
-      <c r="M70" s="25"/>
-      <c r="N70" s="25"/>
-    </row>
-    <row r="71" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K71" s="25"/>
-      <c r="L71" s="25"/>
-      <c r="M71" s="25"/>
-      <c r="N71" s="25"/>
-    </row>
-    <row r="72" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K72" s="25"/>
-      <c r="L72" s="25"/>
-      <c r="M72" s="25"/>
-      <c r="N72" s="25"/>
-    </row>
-    <row r="73" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K73" s="25"/>
-      <c r="L73" s="25"/>
-      <c r="M73" s="25"/>
-      <c r="N73" s="25"/>
-    </row>
-    <row r="74" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K74" s="25"/>
-      <c r="L74" s="25"/>
-      <c r="M74" s="25"/>
-      <c r="N74" s="25"/>
-    </row>
-    <row r="75" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K75" s="25"/>
-      <c r="L75" s="25"/>
-      <c r="M75" s="25"/>
-      <c r="N75" s="25"/>
-    </row>
-    <row r="76" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K76" s="25"/>
-      <c r="L76" s="25"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
-    </row>
-    <row r="77" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K77" s="25"/>
-      <c r="L77" s="25"/>
-      <c r="M77" s="25"/>
-      <c r="N77" s="25"/>
-    </row>
-    <row r="78" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K78" s="25"/>
-      <c r="L78" s="25"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="25"/>
-    </row>
-    <row r="79" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K79" s="25"/>
-      <c r="L79" s="25"/>
-      <c r="M79" s="25"/>
-      <c r="N79" s="25"/>
-    </row>
-    <row r="80" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K80" s="25"/>
-      <c r="L80" s="25"/>
-      <c r="M80" s="25"/>
-      <c r="N80" s="25"/>
-    </row>
-    <row r="81" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K81" s="25"/>
-      <c r="L81" s="25"/>
-      <c r="M81" s="25"/>
-      <c r="N81" s="25"/>
-    </row>
-    <row r="82" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K82" s="25"/>
-      <c r="L82" s="25"/>
-      <c r="M82" s="25"/>
-      <c r="N82" s="25"/>
-    </row>
-    <row r="83" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K83" s="25"/>
-      <c r="L83" s="25"/>
-      <c r="M83" s="25"/>
-      <c r="N83" s="25"/>
-    </row>
-    <row r="84" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K84" s="25"/>
-      <c r="L84" s="25"/>
-      <c r="M84" s="25"/>
-      <c r="N84" s="25"/>
-    </row>
-    <row r="85" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K85" s="25"/>
-      <c r="L85" s="25"/>
-      <c r="M85" s="25"/>
-      <c r="N85" s="25"/>
-    </row>
-    <row r="86" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K86" s="25"/>
-      <c r="L86" s="25"/>
-      <c r="M86" s="25"/>
-      <c r="N86" s="25"/>
-    </row>
-    <row r="87" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K87" s="25"/>
-      <c r="L87" s="25"/>
-      <c r="M87" s="25"/>
-      <c r="N87" s="25"/>
-    </row>
-    <row r="88" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K88" s="25"/>
-      <c r="L88" s="25"/>
-      <c r="M88" s="25"/>
-      <c r="N88" s="25"/>
-    </row>
-    <row r="89" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K89" s="25"/>
-      <c r="L89" s="25"/>
-      <c r="M89" s="25"/>
-      <c r="N89" s="25"/>
-    </row>
-    <row r="90" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K90" s="25"/>
-      <c r="L90" s="25"/>
-      <c r="M90" s="25"/>
-      <c r="N90" s="25"/>
-    </row>
-    <row r="91" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K91" s="25"/>
-      <c r="L91" s="25"/>
-      <c r="M91" s="25"/>
-      <c r="N91" s="25"/>
-    </row>
-    <row r="92" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K92" s="25"/>
-      <c r="L92" s="25"/>
-      <c r="M92" s="25"/>
-      <c r="N92" s="25"/>
-    </row>
-    <row r="93" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K93" s="25"/>
-      <c r="L93" s="25"/>
-      <c r="M93" s="25"/>
-      <c r="N93" s="25"/>
-    </row>
-    <row r="94" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K94" s="25"/>
-      <c r="L94" s="25"/>
-      <c r="M94" s="25"/>
-      <c r="N94" s="25"/>
-    </row>
-    <row r="95" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K95" s="25"/>
-      <c r="L95" s="25"/>
-      <c r="M95" s="25"/>
-      <c r="N95" s="25"/>
-    </row>
-    <row r="96" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K96" s="25"/>
-      <c r="L96" s="25"/>
-      <c r="M96" s="25"/>
-      <c r="N96" s="25"/>
-    </row>
-    <row r="97" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K97" s="25"/>
-      <c r="L97" s="25"/>
-      <c r="M97" s="25"/>
-      <c r="N97" s="25"/>
-    </row>
-    <row r="98" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K98" s="25"/>
-      <c r="L98" s="25"/>
-      <c r="M98" s="25"/>
-      <c r="N98" s="25"/>
-    </row>
-    <row r="99" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K99" s="25"/>
-      <c r="L99" s="25"/>
-      <c r="M99" s="25"/>
-      <c r="N99" s="25"/>
-    </row>
-    <row r="100" spans="11:14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="K100" s="25"/>
-      <c r="L100" s="25"/>
-      <c r="M100" s="25"/>
-      <c r="N100" s="25"/>
-    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>150</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>192</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>200</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A11:J11"/>

</xml_diff>